<commit_message>
New update of data
</commit_message>
<xml_diff>
--- a/data/Ireland.xlsx
+++ b/data/Ireland.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="80">
   <si>
     <t xml:space="preserve">Province.State</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t xml:space="preserve">2020-03-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-03-31</t>
   </si>
 </sst>
 </file>
@@ -365,7 +368,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.95"/>
@@ -1494,13 +1497,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G139"/>
+  <dimension ref="A1:G141"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A112" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E140" activeCellId="0" sqref="E140"/>
+      <selection pane="topLeft" activeCell="F142" activeCellId="0" sqref="F142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.95"/>
@@ -4297,6 +4300,46 @@
         <v>63</v>
       </c>
     </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B140" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C140" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D140" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F140" s="0" t="n">
+        <v>325</v>
+      </c>
+      <c r="G140" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B141" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C141" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D141" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F141" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G141" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added HPSC data, and updated predictions
</commit_message>
<xml_diff>
--- a/data/Ireland.xlsx
+++ b/data/Ireland.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="90">
   <si>
     <t xml:space="preserve">Province.State</t>
   </si>
@@ -261,6 +261,36 @@
   </si>
   <si>
     <t xml:space="preserve">2020-03-31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-10</t>
   </si>
 </sst>
 </file>
@@ -365,10 +395,10 @@
   <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A162:G163 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.95"/>
@@ -1497,13 +1527,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G141"/>
+  <dimension ref="A1:G163"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A112" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F142" activeCellId="0" sqref="F142"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A133" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A162" activeCellId="0" sqref="A162:G163"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.95"/>
@@ -4340,6 +4370,412 @@
         <v>63</v>
       </c>
     </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B142" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C142" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D142" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F142" s="0" t="n">
+        <v>212</v>
+      </c>
+      <c r="G142" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B143" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C143" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D143" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F143" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="G143" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B144" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C144" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D144" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F144" s="0" t="n">
+        <v>402</v>
+      </c>
+      <c r="G144" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B145" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C145" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D145" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F145" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G145" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B146" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C146" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D146" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F146" s="0" t="n">
+        <v>424</v>
+      </c>
+      <c r="G146" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B147" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C147" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D147" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F147" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="G147" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B148" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C148" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D148" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F148" s="0" t="n">
+        <v>331</v>
+      </c>
+      <c r="G148" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B149" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C149" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D149" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F149" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G149" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B150" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C150" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D150" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F150" s="0" t="n">
+        <v>390</v>
+      </c>
+      <c r="G150" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B151" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C151" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D151" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F151" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="G151" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B152" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C152" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D152" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F152" s="0" t="n">
+        <v>370</v>
+      </c>
+      <c r="G152" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B153" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C153" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D153" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F153" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="G153" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B154" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C154" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D154" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F154" s="0" t="n">
+        <v>345</v>
+      </c>
+      <c r="G154" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B155" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C155" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D155" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F155" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="G155" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B156" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C156" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D156" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F156" s="0" t="n">
+        <v>365</v>
+      </c>
+      <c r="G156" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B157" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C157" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D157" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F157" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="G157" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B158" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C158" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D158" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F158" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="G158" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B159" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C159" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D159" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F159" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="G159" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B160" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C160" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D160" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F160" s="0" t="n">
+        <v>480</v>
+      </c>
+      <c r="G160" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B161" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C161" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D161" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F161" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="G161" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E162" s="1"/>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E163" s="1"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added commentary to the R0 Rmd file Some new images and HPSC files too.
</commit_message>
<xml_diff>
--- a/data/Ireland.xlsx
+++ b/data/Ireland.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="96">
   <si>
     <t xml:space="preserve">Province.State</t>
   </si>
@@ -291,6 +291,24 @@
   </si>
   <si>
     <t xml:space="preserve">2020-04-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-16</t>
   </si>
 </sst>
 </file>
@@ -395,10 +413,10 @@
   <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A162:G163 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.95"/>
@@ -1527,13 +1545,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G163"/>
+  <dimension ref="A1:G173"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A133" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A162" activeCellId="0" sqref="A162:G163"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A137" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F172" activeCellId="0" sqref="F172"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.95"/>
@@ -4771,10 +4789,244 @@
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E162" s="1"/>
+      <c r="B162" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C162" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D162" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F162" s="0" t="n">
+        <v>553</v>
+      </c>
+      <c r="G162" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E163" s="1"/>
+      <c r="B163" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C163" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D163" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F163" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="G163" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B164" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C164" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D164" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F164" s="0" t="n">
+        <v>430</v>
+      </c>
+      <c r="G164" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B165" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C165" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D165" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F165" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="G165" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B166" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C166" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D166" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F166" s="0" t="n">
+        <v>527</v>
+      </c>
+      <c r="G166" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B167" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C167" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D167" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F167" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="G167" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B168" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C168" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D168" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F168" s="0" t="n">
+        <v>548</v>
+      </c>
+      <c r="G168" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B169" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C169" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D169" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F169" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="G169" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B170" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C170" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D170" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F170" s="0" t="n">
+        <v>657</v>
+      </c>
+      <c r="G170" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B171" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C171" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D171" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F171" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="G171" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B172" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C172" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D172" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F172" s="0" t="n">
+        <v>629</v>
+      </c>
+      <c r="G172" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B173" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C173" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D173" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F173" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="G173" s="0" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Update to data for April 26th
</commit_message>
<xml_diff>
--- a/data/Ireland.xlsx
+++ b/data/Ireland.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="106">
   <si>
     <t xml:space="preserve">Province.State</t>
   </si>
@@ -309,6 +309,36 @@
   </si>
   <si>
     <t xml:space="preserve">2020-04-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-26</t>
   </si>
 </sst>
 </file>
@@ -416,7 +446,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.95"/>
@@ -1545,13 +1575,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G173"/>
+  <dimension ref="A1:G193"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A137" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F172" activeCellId="0" sqref="F172"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F192" activeCellId="0" sqref="F192"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.95"/>
@@ -5028,6 +5058,406 @@
         <v>63</v>
       </c>
     </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B174" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C174" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D174" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F174" s="0" t="n">
+        <v>597</v>
+      </c>
+      <c r="G174" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B175" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C175" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D175" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F175" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="G175" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B176" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C176" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D176" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F176" s="0" t="n">
+        <v>630</v>
+      </c>
+      <c r="G176" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B177" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C177" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D177" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F177" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="G177" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B178" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C178" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D178" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F178" s="0" t="n">
+        <v>445</v>
+      </c>
+      <c r="G178" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B179" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C179" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D179" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F179" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="G179" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B180" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C180" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D180" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F180" s="0" t="n">
+        <v>401</v>
+      </c>
+      <c r="G180" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B181" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C181" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D181" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F181" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="G181" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B182" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C182" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D182" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F182" s="0" t="n">
+        <v>388</v>
+      </c>
+      <c r="G182" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B183" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C183" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D183" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F183" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="G183" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B184" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C184" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D184" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F184" s="0" t="n">
+        <v>631</v>
+      </c>
+      <c r="G184" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B185" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C185" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D185" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F185" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="G185" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B186" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C186" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D186" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F186" s="0" t="n">
+        <v>936</v>
+      </c>
+      <c r="G186" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B187" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C187" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D187" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F187" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="G187" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B188" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C188" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D188" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F188" s="0" t="n">
+        <v>577</v>
+      </c>
+      <c r="G188" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B189" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C189" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D189" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F189" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="G189" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B190" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C190" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D190" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F190" s="0" t="n">
+        <v>377</v>
+      </c>
+      <c r="G190" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B191" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C191" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D191" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F191" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="G191" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B192" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C192" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D192" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F192" s="0" t="n">
+        <v>701</v>
+      </c>
+      <c r="G192" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B193" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C193" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D193" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F193" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="G193" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Update of data and minor edits to file
</commit_message>
<xml_diff>
--- a/data/Ireland.xlsx
+++ b/data/Ireland.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="108">
   <si>
     <t xml:space="preserve">Province.State</t>
   </si>
@@ -339,6 +339,12 @@
   </si>
   <si>
     <t xml:space="preserve">2020-04-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-04-28</t>
   </si>
 </sst>
 </file>
@@ -446,7 +452,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.95"/>
@@ -1575,13 +1581,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G193"/>
+  <dimension ref="A1:G197"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F192" activeCellId="0" sqref="F192"/>
+      <selection pane="topLeft" activeCell="F198" activeCellId="0" sqref="F198"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.95"/>
@@ -5458,6 +5464,86 @@
         <v>63</v>
       </c>
     </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B194" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C194" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D194" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F194" s="0" t="n">
+        <v>386</v>
+      </c>
+      <c r="G194" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B195" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C195" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D195" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F195" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="G195" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B196" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C196" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D196" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F196" s="0" t="n">
+        <v>229</v>
+      </c>
+      <c r="G196" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B197" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C197" s="0" t="n">
+        <v>53.1424</v>
+      </c>
+      <c r="D197" s="0" t="n">
+        <v>-7.6921</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F197" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="G197" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>